<commit_message>
Working on sequence recorder
</commit_message>
<xml_diff>
--- a/TouchGFX/assets/texts/texts.xlsx
+++ b/TouchGFX/assets/texts/texts.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="356" uniqueCount="63">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="406" uniqueCount="65">
   <si>
     <t xml:space="preserve">Font</t>
   </si>
@@ -213,6 +213,12 @@
   </si>
   <si>
     <t xml:space="preserve">Base</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId6</t>
+  </si>
+  <si>
+    <t xml:space="preserve">&lt;value&gt;</t>
   </si>
 </sst>
 </file>
@@ -1758,6 +1764,23 @@
         <v>62</v>
       </c>
     </row>
+    <row r="9">
+      <c r="B9" t="s">
+        <v>63</v>
+      </c>
+      <c r="C9" t="s">
+        <v>38</v>
+      </c>
+      <c r="D9" t="s">
+        <v>48</v>
+      </c>
+      <c r="E9" t="s">
+        <v>44</v>
+      </c>
+      <c r="F9" t="s">
+        <v>64</v>
+      </c>
+    </row>
   </sheetData>
   <mergeCells count="1">
     <mergeCell ref="B2:E2"/>

</xml_diff>

<commit_message>
Added working scroll list
</commit_message>
<xml_diff>
--- a/TouchGFX/assets/texts/texts.xlsx
+++ b/TouchGFX/assets/texts/texts.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="580" uniqueCount="70">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1488" uniqueCount="82">
   <si>
     <t xml:space="preserve">Font</t>
   </si>
@@ -234,6 +234,42 @@
   </si>
   <si>
     <t xml:space="preserve">TEST</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0-9,a-z,A-Z</t>
+  </si>
+  <si>
+    <t xml:space="preserve">?!,</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId10</t>
+  </si>
+  <si>
+    <t xml:space="preserve">INFO</t>
+  </si>
+  <si>
+    <t xml:space="preserve">INFO:</t>
+  </si>
+  <si>
+    <t xml:space="preserve">?!, :</t>
+  </si>
+  <si>
+    <t xml:space="preserve">!@#$%^&amp;*()_+-=,.&lt;&gt;;':"[]{}\|`~</t>
+  </si>
+  <si>
+    <t xml:space="preserve">!@#$%^&amp;*()_+-=,.&lt;&gt;;':"[]{}\|`~ </t>
+  </si>
+  <si>
+    <t xml:space="preserve">GB-DIRECTION</t>
+  </si>
+  <si>
+    <t xml:space="preserve">GB-ALIGNMENT</t>
+  </si>
+  <si>
+    <t xml:space="preserve">GB-TYPOGRAPHY</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0-9,a-z,A-Z,0x20</t>
   </si>
 </sst>
 </file>
@@ -1475,9 +1511,13 @@
       <c r="F4" t="s">
         <v>17</v>
       </c>
-      <c r="G4"/>
+      <c r="G4" t="s">
+        <v>76</v>
+      </c>
       <c r="H4"/>
-      <c r="I4"/>
+      <c r="I4" t="s">
+        <v>81</v>
+      </c>
       <c r="J4"/>
       <c r="L4" s="4" t="s">
         <v>9</v>
@@ -1545,9 +1585,13 @@
       <c r="F6" t="s">
         <v>17</v>
       </c>
-      <c r="G6"/>
+      <c r="G6" t="s">
+        <v>76</v>
+      </c>
       <c r="H6"/>
-      <c r="I6"/>
+      <c r="I6" t="s">
+        <v>81</v>
+      </c>
       <c r="J6"/>
       <c r="L6" s="7" t="s">
         <v>2</v>
@@ -1693,6 +1737,15 @@
       <c r="F3" t="s">
         <v>36</v>
       </c>
+      <c r="G3" t="s">
+        <v>78</v>
+      </c>
+      <c r="H3" t="s">
+        <v>79</v>
+      </c>
+      <c r="I3" t="s">
+        <v>80</v>
+      </c>
     </row>
     <row r="4">
       <c r="B4" t="s">
@@ -1784,7 +1837,7 @@
         <v>63</v>
       </c>
       <c r="C9" t="s">
-        <v>38</v>
+        <v>41</v>
       </c>
       <c r="D9" t="s">
         <v>48</v>
@@ -1828,6 +1881,32 @@
       </c>
       <c r="F11" t="s">
         <v>69</v>
+      </c>
+    </row>
+    <row r="12">
+      <c r="B12" t="s">
+        <v>72</v>
+      </c>
+      <c r="C12" t="s">
+        <v>41</v>
+      </c>
+      <c r="D12" t="s">
+        <v>43</v>
+      </c>
+      <c r="E12" t="s">
+        <v>44</v>
+      </c>
+      <c r="F12" t="s">
+        <v>74</v>
+      </c>
+      <c r="G12" t="s">
+        <v>44</v>
+      </c>
+      <c r="H12" t="s">
+        <v>48</v>
+      </c>
+      <c r="I12" t="s">
+        <v>41</v>
       </c>
     </row>
   </sheetData>

</xml_diff>